<commit_message>
Completed Tier 1 Backend
</commit_message>
<xml_diff>
--- a/utilities/Carmichael Planning Sheet.xlsx
+++ b/utilities/Carmichael Planning Sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="14880" tabRatio="500"/>
+    <workbookView xWindow="40" yWindow="440" windowWidth="19600" windowHeight="14540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>Tier 1 Goal - Dashboard</t>
   </si>
@@ -59,15 +59,12 @@
     <t>Redux</t>
   </si>
   <si>
-    <t xml:space="preserve">  Dashboard</t>
+    <t>Dashboard</t>
   </si>
   <si>
     <t>GetAll</t>
   </si>
   <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>GetAllByType</t>
   </si>
   <si>
@@ -101,18 +98,9 @@
     <t>Orders</t>
   </si>
   <si>
-    <t>Ratios - Segment Inventory Turnover</t>
-  </si>
-  <si>
-    <t>Ratios - Inventory Turnover, Demand Overview</t>
-  </si>
-  <si>
     <t>Ratios - Segment By Demand</t>
   </si>
   <si>
-    <t xml:space="preserve">  Orders with GPM</t>
-  </si>
-  <si>
     <t>^</t>
   </si>
   <si>
@@ -321,12 +309,6 @@
     <t>D3js/Sheetjs</t>
   </si>
   <si>
-    <t>Sheetjs/D3js</t>
-  </si>
-  <si>
-    <t>threejs</t>
-  </si>
-  <si>
     <t>Ability to make it into mobile app</t>
   </si>
   <si>
@@ -334,6 +316,36 @@
   </si>
   <si>
     <t>"Tech is about pushing yourself"</t>
+  </si>
+  <si>
+    <t>Seed</t>
+  </si>
+  <si>
+    <t>Product, Categories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Overview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Inventory</t>
+  </si>
+  <si>
+    <t>GeneralLedger</t>
+  </si>
+  <si>
+    <t>GetAll, GetAllByType</t>
+  </si>
+  <si>
+    <t>Inventory Turnover (Sales / Inventory), Inventory Write-Off (Discontinued / Inventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Customer</t>
+  </si>
+  <si>
+    <t>Segmentation, Demand, Gross Profit</t>
+  </si>
+  <si>
+    <t>GrossProfit, NetProfit</t>
   </si>
 </sst>
 </file>
@@ -383,7 +395,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,10 +414,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I38"/>
+  <dimension ref="A2:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -720,224 +732,245 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>40</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
         <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="1"/>
+      <c r="H7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>43</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
       </c>
       <c r="I9" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="I12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>43</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="I21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="2"/>
+      <c r="B36" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+      <c r="B38" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="3"/>
-      <c r="B34" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>